<commit_message>
Added CSVs and updated data lists
</commit_message>
<xml_diff>
--- a/inst/extdata/DataFromOtherPackages.xlsx
+++ b/inst/extdata/DataFromOtherPackages.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="160">
   <si>
     <t>Dataset</t>
   </si>
@@ -147,10 +147,6 @@
     <t>Capture-Recapture</t>
   </si>
   <si>
-    <t>The complete capture histories of striped bass for Lake
-Gaston, North Carolina</t>
-  </si>
-  <si>
     <t>Jensen</t>
   </si>
   <si>
@@ -217,9 +213,6 @@
     <t>rockbass</t>
   </si>
   <si>
-    <t>The age data are from a sample of rock bass trap-netted from Cayuga Lake, New York by Chapman and Robson, as reported by Seber (2002; page 417) and were expanded to individual observations from the age frequency table</t>
-  </si>
-  <si>
     <t>sblen</t>
   </si>
   <si>
@@ -257,9 +250,6 @@
   </si>
   <si>
     <t>trout</t>
-  </si>
-  <si>
-    <t>Release lengths, recapture lengths and timesat-large for trout trout in the Kenai River from Table 4.10 of Quinn and Deriso (1999)</t>
   </si>
   <si>
     <t>wolffish</t>
@@ -476,6 +466,81 @@
   </si>
   <si>
     <t>Stat2Data</t>
+  </si>
+  <si>
+    <t>The complete capture histories of striped bass for Lake Gaston, North Carolina</t>
+  </si>
+  <si>
+    <t>Age data from a sample of rock bass trap-netted from Cayuga Lake, New York</t>
+  </si>
+  <si>
+    <t>Release lengths, recapture lengths and times-at-large for trout in the Kenai River</t>
+  </si>
+  <si>
+    <t>Catch data for the Tasmanian abalone fishery</t>
+  </si>
+  <si>
+    <t>MQMF</t>
+  </si>
+  <si>
+    <t>abdat</t>
+  </si>
+  <si>
+    <t>blackisland</t>
+  </si>
+  <si>
+    <t>Length from tagging data for blacklip abalone at the Black Island site, Tasmania</t>
+  </si>
+  <si>
+    <t>dataspm</t>
+  </si>
+  <si>
+    <t>Catch data for Pink Ling</t>
+  </si>
+  <si>
+    <t>LatA</t>
+  </si>
+  <si>
+    <t>Simulated age data for redfish from eastern Australia in the 1990s</t>
+  </si>
+  <si>
+    <t>minnow</t>
+  </si>
+  <si>
+    <t>Weekly length measurements of a minnow for use with seasonal growth curves</t>
+  </si>
+  <si>
+    <t>npf</t>
+  </si>
+  <si>
+    <t>Catch data (year, biomass, effort) for several species in the Australian Northern Prawn Fishery</t>
+  </si>
+  <si>
+    <t>pttuna</t>
+  </si>
+  <si>
+    <t>Yellowfin tuna fishery data (catch effort by year) from Pella-Tomlinson 1969</t>
+  </si>
+  <si>
+    <t>schaef</t>
+  </si>
+  <si>
+    <t>Yellowfin tuna fishery data (catch effort by year) from Schaefer 1957</t>
+  </si>
+  <si>
+    <t>tasab</t>
+  </si>
+  <si>
+    <t>Maturity and length data for Blacklip Abalone from Tasmania</t>
+  </si>
+  <si>
+    <t>tigers</t>
+  </si>
+  <si>
+    <t>Prawn recruitment data from Penn and Caputi (1986)</t>
+  </si>
+  <si>
+    <t>Recruitment</t>
   </si>
 </sst>
 </file>
@@ -975,10 +1040,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1300,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59:F60"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62:F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1356,7 +1419,7 @@
         <v>44885</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1376,7 +1439,7 @@
         <v>44885</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1396,7 +1459,7 @@
         <v>44885</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1420,7 +1483,7 @@
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
@@ -1440,7 +1503,7 @@
       <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C7" t="s">
@@ -1460,7 +1523,7 @@
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
@@ -1480,7 +1543,7 @@
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C9" t="s">
@@ -1500,7 +1563,7 @@
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C10" t="s">
@@ -1520,7 +1583,7 @@
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" t="s">
@@ -1540,7 +1603,7 @@
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C12" t="s">
@@ -1560,7 +1623,7 @@
       <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" t="s">
@@ -1576,12 +1639,12 @@
         <v>44885</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
@@ -1598,10 +1661,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>37</v>
@@ -1618,10 +1681,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1638,10 +1701,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1658,10 +1721,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
         <v>49</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
@@ -1678,13 +1741,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
@@ -1698,10 +1761,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
@@ -1718,10 +1781,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
         <v>56</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -1738,10 +1801,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" t="s">
         <v>58</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1758,10 +1821,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1778,10 +1841,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" t="s">
         <v>62</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -1798,10 +1861,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="C25" t="s">
         <v>37</v>
@@ -1818,13 +1881,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
         <v>66</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
@@ -1838,13 +1901,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
         <v>69</v>
-      </c>
-      <c r="B27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -1858,13 +1921,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
@@ -1878,10 +1941,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -1898,10 +1961,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
@@ -1918,10 +1981,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C31" t="s">
         <v>20</v>
@@ -1938,10 +2001,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -1958,10 +2021,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C33" t="s">
         <v>20</v>
@@ -1978,10 +2041,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="C34" t="s">
         <v>20</v>
@@ -1998,16 +2061,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -2016,38 +2079,38 @@
         <v>44885</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
       <c r="D36" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="1">
+        <v>44885</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>86</v>
       </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="1">
-        <v>44885</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>89</v>
-      </c>
       <c r="B37" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E37" t="s">
         <v>10</v>
@@ -2058,16 +2121,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E38" t="s">
         <v>10</v>
@@ -2078,16 +2141,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -2098,16 +2161,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -2118,16 +2181,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" t="s">
-        <v>97</v>
+        <v>93</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="C41" t="s">
         <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -2138,16 +2201,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B42" t="s">
-        <v>101</v>
-      </c>
       <c r="C42" t="s">
         <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -2158,16 +2221,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>99</v>
-      </c>
-      <c r="B43" t="s">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="C43" t="s">
         <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -2178,16 +2241,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" t="s">
-        <v>103</v>
+        <v>99</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C44" t="s">
         <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -2200,14 +2263,14 @@
       <c r="A45" t="s">
         <v>38</v>
       </c>
-      <c r="B45" t="s">
-        <v>104</v>
+      <c r="B45" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="C45" t="s">
         <v>20</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -2218,16 +2281,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>105</v>
-      </c>
-      <c r="B46" t="s">
-        <v>106</v>
+        <v>102</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="C46" t="s">
         <v>20</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -2238,16 +2301,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>107</v>
-      </c>
-      <c r="B47" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="C47" t="s">
         <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E47" t="s">
         <v>10</v>
@@ -2258,16 +2321,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>109</v>
-      </c>
-      <c r="B48" t="s">
-        <v>110</v>
+        <v>106</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="C48" t="s">
         <v>20</v>
       </c>
       <c r="D48" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
@@ -2278,16 +2341,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>111</v>
-      </c>
-      <c r="B49" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C49" t="s">
         <v>37</v>
       </c>
       <c r="D49" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
@@ -2298,16 +2361,16 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C50" t="s">
         <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
@@ -2318,16 +2381,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="C51" t="s">
         <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
@@ -2338,16 +2401,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
@@ -2358,16 +2421,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" t="s">
         <v>125</v>
-      </c>
-      <c r="B53" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" t="s">
-        <v>20</v>
-      </c>
-      <c r="D53" t="s">
-        <v>128</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
@@ -2378,16 +2441,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>126</v>
-      </c>
-      <c r="B54" t="s">
-        <v>119</v>
+        <v>123</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D54" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>
@@ -2398,16 +2461,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>127</v>
-      </c>
-      <c r="B55" t="s">
-        <v>120</v>
+        <v>124</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E55" t="s">
         <v>10</v>
@@ -2418,16 +2481,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" t="s">
-        <v>122</v>
+        <v>118</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C56" t="s">
         <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E56" t="s">
         <v>10</v>
@@ -2438,16 +2501,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>123</v>
-      </c>
-      <c r="B57" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="C57" t="s">
         <v>20</v>
       </c>
       <c r="D57" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E57" t="s">
         <v>10</v>
@@ -2458,16 +2521,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>129</v>
-      </c>
-      <c r="B58" t="s">
-        <v>130</v>
+        <v>126</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C58" t="s">
         <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E58" t="s">
         <v>10</v>
@@ -2478,16 +2541,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
         <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E59" t="s">
         <v>10</v>
@@ -2498,22 +2561,222 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D60" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E60" t="s">
         <v>10</v>
       </c>
       <c r="F60" s="1">
         <v>44885</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" t="s">
+        <v>139</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" t="s">
+        <v>139</v>
+      </c>
+      <c r="E63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>145</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" t="s">
+        <v>139</v>
+      </c>
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" t="s">
+        <v>139</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>149</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" t="s">
+        <v>139</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" t="s">
+        <v>139</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>139</v>
+      </c>
+      <c r="E68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C69" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69" t="s">
+        <v>139</v>
+      </c>
+      <c r="E69" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="1">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C70" t="s">
+        <v>159</v>
+      </c>
+      <c r="D70" t="s">
+        <v>139</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="1">
+        <v>44887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>